<commit_message>
Added seperate train function
</commit_message>
<xml_diff>
--- a/models/Bi-LSTM_Road_Fines_u=32_e=inf/training_metrics.xlsx
+++ b/models/Bi-LSTM_Road_Fines_u=32_e=inf/training_metrics.xlsx
@@ -600,97 +600,97 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.4293261766433716</v>
+        <v>0.5232980847358704</v>
       </c>
       <c r="C2" t="n">
-        <v>2.938307523727417</v>
+        <v>2.709017276763916</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4061579704284668</v>
+        <v>0.4522778391838074</v>
       </c>
       <c r="E2" t="n">
-        <v>2.971457004547119</v>
+        <v>3.056704521179199</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3598648905754089</v>
+        <v>0.4223107695579529</v>
       </c>
       <c r="G2" t="n">
-        <v>3.05966854095459</v>
+        <v>3.020390510559082</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3412870168685913</v>
+        <v>0.3550580143928528</v>
       </c>
       <c r="I2" t="n">
-        <v>3.238869667053223</v>
+        <v>3.237790584564209</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4903862774372101</v>
+        <v>0.54347825050354</v>
       </c>
       <c r="K2" t="n">
-        <v>2.827231884002686</v>
+        <v>2.821513414382935</v>
       </c>
       <c r="L2" t="n">
-        <v>0.4469946324825287</v>
+        <v>0.4821583330631256</v>
       </c>
       <c r="M2" t="n">
-        <v>2.717112302780151</v>
+        <v>3.039693117141724</v>
       </c>
       <c r="N2" t="n">
-        <v>0.4817685782909393</v>
+        <v>0.5365927815437317</v>
       </c>
       <c r="O2" t="n">
-        <v>2.819586277008057</v>
+        <v>2.578890562057495</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4192793965339661</v>
+        <v>0.5165425539016724</v>
       </c>
       <c r="Q2" t="n">
-        <v>2.883475303649902</v>
+        <v>2.82404613494873</v>
       </c>
       <c r="R2" t="n">
-        <v>0.3606876730918884</v>
+        <v>0.5649142265319824</v>
       </c>
       <c r="S2" t="n">
-        <v>3.050355672836304</v>
+        <v>2.681746244430542</v>
       </c>
       <c r="T2" t="n">
-        <v>0.4653559625148773</v>
+        <v>0.5009527206420898</v>
       </c>
       <c r="U2" t="n">
-        <v>2.745136022567749</v>
+        <v>2.894340753555298</v>
       </c>
       <c r="V2" t="n">
-        <v>0.465312659740448</v>
+        <v>0.5574657917022705</v>
       </c>
       <c r="W2" t="n">
-        <v>2.980398654937744</v>
+        <v>2.610142230987549</v>
       </c>
       <c r="X2" t="n">
-        <v>0.5206565260887146</v>
+        <v>0.5297072529792786</v>
       </c>
       <c r="Y2" t="n">
-        <v>2.612415790557861</v>
+        <v>2.833125591278076</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.4644898772239685</v>
+        <v>0.5851377248764038</v>
       </c>
       <c r="AA2" t="n">
-        <v>2.761622428894043</v>
+        <v>2.72585916519165</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.4868352711200714</v>
+        <v>0.5334748029708862</v>
       </c>
       <c r="AC2" t="n">
-        <v>2.751283168792725</v>
+        <v>2.744796514511108</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.5015156865119934</v>
+        <v>0.5152000784873962</v>
       </c>
       <c r="AE2" t="n">
-        <v>2.967885971069336</v>
+        <v>2.862178325653076</v>
       </c>
       <c r="AF2" t="n">
-        <v>43.32479476928711</v>
+        <v>42.6402473449707</v>
       </c>
     </row>
     <row r="3">
@@ -698,97 +698,97 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8202840685844421</v>
+        <v>0.824701189994812</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5839772820472717</v>
+        <v>0.5300958752632141</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6446821689605713</v>
+        <v>0.6448986530303955</v>
       </c>
       <c r="E3" t="n">
-        <v>1.136882424354553</v>
+        <v>1.110059261322021</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7573185563087463</v>
+        <v>0.7622120380401611</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8304648399353027</v>
+        <v>0.7923889756202698</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6106444001197815</v>
+        <v>0.61168372631073</v>
       </c>
       <c r="I3" t="n">
-        <v>1.17909038066864</v>
+        <v>1.142401099205017</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8255673050880432</v>
+        <v>0.8251775503158569</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5877169966697693</v>
+        <v>0.5393660664558411</v>
       </c>
       <c r="L3" t="n">
-        <v>0.815477192401886</v>
+        <v>0.8227957487106323</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5889877080917358</v>
+        <v>0.5907964706420898</v>
       </c>
       <c r="N3" t="n">
-        <v>0.8296812772750854</v>
+        <v>0.8232721090316772</v>
       </c>
       <c r="O3" t="n">
-        <v>0.6428507566452026</v>
+        <v>0.6082631349563599</v>
       </c>
       <c r="P3" t="n">
-        <v>0.8160834908485413</v>
+        <v>0.822839081287384</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.5948932766914368</v>
+        <v>0.539411723613739</v>
       </c>
       <c r="R3" t="n">
-        <v>0.777498722076416</v>
+        <v>0.7875887751579285</v>
       </c>
       <c r="S3" t="n">
-        <v>0.7301959991455078</v>
+        <v>0.6492300033569336</v>
       </c>
       <c r="T3" t="n">
-        <v>0.822882354259491</v>
+        <v>0.8213667273521423</v>
       </c>
       <c r="U3" t="n">
-        <v>0.5886327624320984</v>
+        <v>0.5737504959106445</v>
       </c>
       <c r="V3" t="n">
-        <v>0.7927420735359192</v>
+        <v>0.7985449433326721</v>
       </c>
       <c r="W3" t="n">
-        <v>0.6893183588981628</v>
+        <v>0.6190176606178284</v>
       </c>
       <c r="X3" t="n">
         <v>0.8231855034828186</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.5531278252601624</v>
+        <v>0.5296198129653931</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.8284687399864197</v>
+        <v>0.8292482495307922</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.581699550151825</v>
+        <v>0.5291793942451477</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.8298544883728027</v>
+        <v>0.8248744010925293</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.6517965197563171</v>
+        <v>0.6159378290176392</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.8157803416252136</v>
+        <v>0.8282955288887024</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.5926434993743896</v>
+        <v>0.5404333472251892</v>
       </c>
       <c r="AF3" t="n">
-        <v>10.53228378295898</v>
+        <v>9.909952163696289</v>
       </c>
     </row>
     <row r="4">
@@ -796,97 +796,97 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8319764137268066</v>
+        <v>0.8359605073928833</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3713566362857819</v>
+        <v>0.3564878106117249</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6564177870750427</v>
+        <v>0.6538628339767456</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9410696029663086</v>
+        <v>0.9263015985488892</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7721721529960632</v>
+        <v>0.7723886966705322</v>
       </c>
       <c r="G4" t="n">
-        <v>0.6059903502464294</v>
+        <v>0.5942257046699524</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6268837451934814</v>
+        <v>0.6293521523475647</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9591795802116394</v>
+        <v>0.9403344392776489</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8325827121734619</v>
+        <v>0.8347912430763245</v>
       </c>
       <c r="K4" t="n">
-        <v>0.373916357755661</v>
+        <v>0.3576248586177826</v>
       </c>
       <c r="L4" t="n">
-        <v>0.8307206034660339</v>
+        <v>0.8379958271980286</v>
       </c>
       <c r="M4" t="n">
-        <v>0.3797001242637634</v>
+        <v>0.3619590997695923</v>
       </c>
       <c r="N4" t="n">
-        <v>0.842759370803833</v>
+        <v>0.8434956073760986</v>
       </c>
       <c r="O4" t="n">
-        <v>0.4381659924983978</v>
+        <v>0.4229556322097778</v>
       </c>
       <c r="P4" t="n">
-        <v>0.8310237526893616</v>
+        <v>0.8369132280349731</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.3726142942905426</v>
+        <v>0.3551364243030548</v>
       </c>
       <c r="R4" t="n">
-        <v>0.7923956513404846</v>
+        <v>0.7977654337882996</v>
       </c>
       <c r="S4" t="n">
-        <v>0.4966099560260773</v>
+        <v>0.4765941202640533</v>
       </c>
       <c r="T4" t="n">
-        <v>0.832106351852417</v>
+        <v>0.833968460559845</v>
       </c>
       <c r="U4" t="n">
-        <v>0.3756760060787201</v>
+        <v>0.3619384467601776</v>
       </c>
       <c r="V4" t="n">
-        <v>0.8103238940238953</v>
+        <v>0.8115364909172058</v>
       </c>
       <c r="W4" t="n">
-        <v>0.466071218252182</v>
+        <v>0.450566440820694</v>
       </c>
       <c r="X4" t="n">
-        <v>0.8324961066246033</v>
+        <v>0.8365668058395386</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.3728341162204742</v>
+        <v>0.3543886244297028</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.832322895526886</v>
+        <v>0.8367832899093628</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.3743709325790405</v>
+        <v>0.3551085591316223</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.8405941724777222</v>
+        <v>0.8426294922828674</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.4424374997615814</v>
+        <v>0.4256309866905212</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.8317599296569824</v>
+        <v>0.8381257653236389</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.373341977596283</v>
+        <v>0.3539482653141022</v>
       </c>
       <c r="AF4" t="n">
-        <v>7.343333721160889</v>
+        <v>7.093203067779541</v>
       </c>
     </row>
     <row r="5">
@@ -894,97 +894,97 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.8389052748680115</v>
+        <v>0.8409838676452637</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3380007147789001</v>
+        <v>0.3334563970565796</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6588428616523743</v>
+        <v>0.6613546013832092</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9079360365867615</v>
+        <v>0.9001128077507019</v>
       </c>
       <c r="F5" t="n">
-        <v>0.777325451374054</v>
+        <v>0.7780616879463196</v>
       </c>
       <c r="G5" t="n">
-        <v>0.567111074924469</v>
+        <v>0.5657532215118408</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6346786618232727</v>
+        <v>0.6340290904045105</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9171440005302429</v>
+        <v>0.9101560711860657</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8402044177055359</v>
+        <v>0.8415468335151672</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3403329253196716</v>
+        <v>0.334507554769516</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8382556438446045</v>
+        <v>0.8427160978317261</v>
       </c>
       <c r="M5" t="n">
-        <v>0.3441113829612732</v>
+        <v>0.337427169084549</v>
       </c>
       <c r="N5" t="n">
+        <v>0.8464836478233337</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.4020196497440338</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.8433223366737366</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.3322597146034241</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.8012298345565796</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.452781468629837</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.8417201042175293</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.3363668024539948</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.814048171043396</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.4252075552940369</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.8422830700874329</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.3322798609733582</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.8425861597061157</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0.3339123427867889</v>
+      </c>
+      <c r="AB5" t="n">
         <v>0.8451845049858093</v>
       </c>
-      <c r="O5" t="n">
-        <v>0.405972421169281</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.8412437438964844</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.3375924229621887</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.7975922226905823</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.4598523676395416</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0.8380391597747803</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.3421240448951721</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0.8133119940757751</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0.4303396046161652</v>
-      </c>
-      <c r="X5" t="n">
-        <v>0.8386453986167908</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0.3381824195384979</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0.8382123708724976</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>0.339313805103302</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0.8448813557624817</v>
-      </c>
       <c r="AC5" t="n">
-        <v>0.4078893661499023</v>
+        <v>0.4042204916477203</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.8384289145469666</v>
+        <v>0.8415468335151672</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.3386723697185516</v>
+        <v>0.3322315812110901</v>
       </c>
       <c r="AF5" t="n">
-        <v>6.814576148986816</v>
+        <v>6.732691287994385</v>
       </c>
     </row>
     <row r="6">
@@ -992,97 +992,97 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8448813557624817</v>
+        <v>0.8430192470550537</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3270532488822937</v>
+        <v>0.3289691209793091</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6613978743553162</v>
+        <v>0.6643859148025513</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8908849358558655</v>
+        <v>0.8918812870979309</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7822622656822205</v>
+        <v>0.7792742252349854</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5497938990592957</v>
+        <v>0.5582778453826904</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6391823887825012</v>
+        <v>0.63831627368927</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9018368721008301</v>
+        <v>0.9025792479515076</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8442750573158264</v>
+        <v>0.8424995541572571</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3286223709583282</v>
+        <v>0.3293662071228027</v>
       </c>
       <c r="L6" t="n">
-        <v>0.8418933153152466</v>
+        <v>0.84340900182724</v>
       </c>
       <c r="M6" t="n">
-        <v>0.3333477675914764</v>
+        <v>0.3339523375034332</v>
       </c>
       <c r="N6" t="n">
-        <v>0.8483890295028687</v>
+        <v>0.8479126691818237</v>
       </c>
       <c r="O6" t="n">
-        <v>0.3908111751079559</v>
+        <v>0.3986920416355133</v>
       </c>
       <c r="P6" t="n">
-        <v>0.8441451787948608</v>
+        <v>0.8432790637016296</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.3267815411090851</v>
+        <v>0.3287070095539093</v>
       </c>
       <c r="R6" t="n">
-        <v>0.8041313290596008</v>
+        <v>0.803178608417511</v>
       </c>
       <c r="S6" t="n">
-        <v>0.4461919963359833</v>
+        <v>0.4481481909751892</v>
       </c>
       <c r="T6" t="n">
-        <v>0.8438853025436401</v>
+        <v>0.8416767716407776</v>
       </c>
       <c r="U6" t="n">
-        <v>0.3310062289237976</v>
+        <v>0.3331458270549774</v>
       </c>
       <c r="V6" t="n">
-        <v>0.8204140067100525</v>
+        <v>0.816126823425293</v>
       </c>
       <c r="W6" t="n">
-        <v>0.4100612699985504</v>
+        <v>0.4213265776634216</v>
       </c>
       <c r="X6" t="n">
-        <v>0.8436688184738159</v>
+        <v>0.8436254858970642</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.3283002376556396</v>
+        <v>0.3274954557418823</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.8435822129249573</v>
+        <v>0.8424995541572571</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.3287509679794312</v>
+        <v>0.3298241794109344</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.8479560017585754</v>
+        <v>0.8474796414375305</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.393433004617691</v>
+        <v>0.3992651700973511</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.8440152406692505</v>
+        <v>0.8425861597061157</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.3276780843734741</v>
+        <v>0.3282879292964935</v>
       </c>
       <c r="AF6" t="n">
-        <v>6.614553451538086</v>
+        <v>6.659918785095215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First Refactoring and renaming of the tool
</commit_message>
<xml_diff>
--- a/models/Bi-LSTM_Road_Fines_u=32_e=inf/training_metrics.xlsx
+++ b/models/Bi-LSTM_Road_Fines_u=32_e=inf/training_metrics.xlsx
@@ -600,97 +600,97 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.5232980847358704</v>
+        <v>0.4946301877498627</v>
       </c>
       <c r="C2" t="n">
-        <v>2.709017276763916</v>
+        <v>2.815833806991577</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4522778391838074</v>
+        <v>0.4332236349582672</v>
       </c>
       <c r="E2" t="n">
-        <v>3.056704521179199</v>
+        <v>3.122532367706299</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4223107695579529</v>
+        <v>0.4092326462268829</v>
       </c>
       <c r="G2" t="n">
-        <v>3.020390510559082</v>
+        <v>3.225309371948242</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3550580143928528</v>
+        <v>0.4020873010158539</v>
       </c>
       <c r="I2" t="n">
-        <v>3.237790584564209</v>
+        <v>3.124607563018799</v>
       </c>
       <c r="J2" t="n">
-        <v>0.54347825050354</v>
+        <v>0.5248571038246155</v>
       </c>
       <c r="K2" t="n">
-        <v>2.821513414382935</v>
+        <v>2.787523746490479</v>
       </c>
       <c r="L2" t="n">
-        <v>0.4821583330631256</v>
+        <v>0.5152433514595032</v>
       </c>
       <c r="M2" t="n">
-        <v>3.039693117141724</v>
+        <v>2.707319021224976</v>
       </c>
       <c r="N2" t="n">
-        <v>0.5365927815437317</v>
+        <v>0.4846267104148865</v>
       </c>
       <c r="O2" t="n">
-        <v>2.578890562057495</v>
+        <v>2.779758453369141</v>
       </c>
       <c r="P2" t="n">
-        <v>0.5165425539016724</v>
+        <v>0.5758704543113708</v>
       </c>
       <c r="Q2" t="n">
-        <v>2.82404613494873</v>
+        <v>2.559982776641846</v>
       </c>
       <c r="R2" t="n">
-        <v>0.5649142265319824</v>
+        <v>0.4107050001621246</v>
       </c>
       <c r="S2" t="n">
-        <v>2.681746244430542</v>
+        <v>3.026839256286621</v>
       </c>
       <c r="T2" t="n">
-        <v>0.5009527206420898</v>
+        <v>0.4933743178844452</v>
       </c>
       <c r="U2" t="n">
-        <v>2.894340753555298</v>
+        <v>2.97681450843811</v>
       </c>
       <c r="V2" t="n">
-        <v>0.5574657917022705</v>
+        <v>0.5273687839508057</v>
       </c>
       <c r="W2" t="n">
-        <v>2.610142230987549</v>
+        <v>2.842788934707642</v>
       </c>
       <c r="X2" t="n">
-        <v>0.5297072529792786</v>
+        <v>0.4992205202579498</v>
       </c>
       <c r="Y2" t="n">
-        <v>2.833125591278076</v>
+        <v>2.821062564849854</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.5851377248764038</v>
+        <v>0.4420578479766846</v>
       </c>
       <c r="AA2" t="n">
-        <v>2.72585916519165</v>
+        <v>2.951903104782104</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.5334748029708862</v>
+        <v>0.4807292520999908</v>
       </c>
       <c r="AC2" t="n">
-        <v>2.744796514511108</v>
+        <v>2.813172578811646</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.5152000784873962</v>
+        <v>0.4832409620285034</v>
       </c>
       <c r="AE2" t="n">
-        <v>2.862178325653076</v>
+        <v>2.875189781188965</v>
       </c>
       <c r="AF2" t="n">
-        <v>42.6402473449707</v>
+        <v>43.43062973022461</v>
       </c>
     </row>
     <row r="3">
@@ -698,97 +698,97 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.824701189994812</v>
+        <v>0.8270396590232849</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5300958752632141</v>
+        <v>0.6224359273910522</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6448986530303955</v>
+        <v>0.6391823887825012</v>
       </c>
       <c r="E3" t="n">
-        <v>1.110059261322021</v>
+        <v>1.184240102767944</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7622120380401611</v>
+        <v>0.7614758610725403</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7923889756202698</v>
+        <v>0.8915688991546631</v>
       </c>
       <c r="H3" t="n">
-        <v>0.61168372631073</v>
+        <v>0.6129395365715027</v>
       </c>
       <c r="I3" t="n">
-        <v>1.142401099205017</v>
+        <v>1.207689881324768</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8251775503158569</v>
+        <v>0.8287285566329956</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5393660664558411</v>
+        <v>0.5969237685203552</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8227957487106323</v>
+        <v>0.8205872178077698</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5907964706420898</v>
+        <v>0.5960666537284851</v>
       </c>
       <c r="N3" t="n">
-        <v>0.8232721090316772</v>
+        <v>0.8364801406860352</v>
       </c>
       <c r="O3" t="n">
-        <v>0.6082631349563599</v>
+        <v>0.6601536870002747</v>
       </c>
       <c r="P3" t="n">
-        <v>0.822839081287384</v>
+        <v>0.8239216804504395</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.539411723613739</v>
+        <v>0.5772038698196411</v>
       </c>
       <c r="R3" t="n">
-        <v>0.7875887751579285</v>
+        <v>0.7815260887145996</v>
       </c>
       <c r="S3" t="n">
-        <v>0.6492300033569336</v>
+        <v>0.7541300654411316</v>
       </c>
       <c r="T3" t="n">
-        <v>0.8213667273521423</v>
+        <v>0.8252641558647156</v>
       </c>
       <c r="U3" t="n">
-        <v>0.5737504959106445</v>
+        <v>0.6244245767593384</v>
       </c>
       <c r="V3" t="n">
-        <v>0.7985449433326721</v>
+        <v>0.8031352758407593</v>
       </c>
       <c r="W3" t="n">
-        <v>0.6190176606178284</v>
+        <v>0.6788083910942078</v>
       </c>
       <c r="X3" t="n">
-        <v>0.8231855034828186</v>
+        <v>0.8272562026977539</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.5296198129653931</v>
+        <v>0.6161686182022095</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.8292482495307922</v>
+        <v>0.8220162987709045</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.5291793942451477</v>
+        <v>0.6207436919212341</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.8248744010925293</v>
+        <v>0.8243980407714844</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.6159378290176392</v>
+        <v>0.6831640005111694</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.8282955288887024</v>
+        <v>0.8262168765068054</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.5404333472251892</v>
+        <v>0.6058982610702515</v>
       </c>
       <c r="AF3" t="n">
-        <v>9.909952163696289</v>
+        <v>10.91961765289307</v>
       </c>
     </row>
     <row r="4">
@@ -796,97 +796,97 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8359605073928833</v>
+        <v>0.8360904455184937</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3564878106117249</v>
+        <v>0.3620176613330841</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6538628339767456</v>
+        <v>0.6539061069488525</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9263015985488892</v>
+        <v>0.9343296885490417</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7723886966705322</v>
+        <v>0.7711328864097595</v>
       </c>
       <c r="G4" t="n">
-        <v>0.5942257046699524</v>
+        <v>0.6043238639831543</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6293521523475647</v>
+        <v>0.6305646896362305</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9403344392776489</v>
+        <v>0.9459807872772217</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8347912430763245</v>
+        <v>0.8373462557792664</v>
       </c>
       <c r="K4" t="n">
-        <v>0.3576248586177826</v>
+        <v>0.3622974157333374</v>
       </c>
       <c r="L4" t="n">
-        <v>0.8379958271980286</v>
+        <v>0.8316299915313721</v>
       </c>
       <c r="M4" t="n">
-        <v>0.3619590997695923</v>
+        <v>0.369905024766922</v>
       </c>
       <c r="N4" t="n">
-        <v>0.8434956073760986</v>
+        <v>0.843192458152771</v>
       </c>
       <c r="O4" t="n">
-        <v>0.4229556322097778</v>
+        <v>0.430520236492157</v>
       </c>
       <c r="P4" t="n">
-        <v>0.8369132280349731</v>
+        <v>0.8340983986854553</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.3551364243030548</v>
+        <v>0.3622550368309021</v>
       </c>
       <c r="R4" t="n">
-        <v>0.7977654337882996</v>
+        <v>0.7938246726989746</v>
       </c>
       <c r="S4" t="n">
-        <v>0.4765941202640533</v>
+        <v>0.4872302114963531</v>
       </c>
       <c r="T4" t="n">
-        <v>0.833968460559845</v>
+        <v>0.8349211812019348</v>
       </c>
       <c r="U4" t="n">
-        <v>0.3619384467601776</v>
+        <v>0.3657464981079102</v>
       </c>
       <c r="V4" t="n">
-        <v>0.8115364909172058</v>
+        <v>0.8095011115074158</v>
       </c>
       <c r="W4" t="n">
-        <v>0.450566440820694</v>
+        <v>0.4549477100372314</v>
       </c>
       <c r="X4" t="n">
-        <v>0.8365668058395386</v>
+        <v>0.8360471129417419</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.3543886244297028</v>
+        <v>0.3635031580924988</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.8367832899093628</v>
+        <v>0.8358305692672729</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.3551085591316223</v>
+        <v>0.361288994550705</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.8426294922828674</v>
+        <v>0.8396847248077393</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.4256309866905212</v>
+        <v>0.4339023530483246</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.8381257653236389</v>
+        <v>0.8351377248764038</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.3539482653141022</v>
+        <v>0.3640555441379547</v>
       </c>
       <c r="AF4" t="n">
-        <v>7.093203067779541</v>
+        <v>7.202302932739258</v>
       </c>
     </row>
     <row r="5">
@@ -894,97 +894,97 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.8409838676452637</v>
+        <v>0.8402044177055359</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3334563970565796</v>
+        <v>0.3396600186824799</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6613546013832092</v>
+        <v>0.6589727997779846</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9001128077507019</v>
+        <v>0.9045972228050232</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7780616879463196</v>
+        <v>0.7752468585968018</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5657532215118408</v>
+        <v>0.5727072358131409</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6340290904045105</v>
+        <v>0.6358045935630798</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9101560711860657</v>
+        <v>0.9157621264457703</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8415468335151672</v>
+        <v>0.8396414518356323</v>
       </c>
       <c r="K5" t="n">
-        <v>0.334507554769516</v>
+        <v>0.3409495651721954</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8427160978317261</v>
+        <v>0.8386453986167908</v>
       </c>
       <c r="M5" t="n">
-        <v>0.337427169084549</v>
+        <v>0.344240128993988</v>
       </c>
       <c r="N5" t="n">
-        <v>0.8464836478233337</v>
+        <v>0.8457041382789612</v>
       </c>
       <c r="O5" t="n">
-        <v>0.4020196497440338</v>
+        <v>0.4035923182964325</v>
       </c>
       <c r="P5" t="n">
-        <v>0.8433223366737366</v>
+        <v>0.8373029828071594</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.3322597146034241</v>
+        <v>0.3401212692260742</v>
       </c>
       <c r="R5" t="n">
-        <v>0.8012298345565796</v>
+        <v>0.7977221608161926</v>
       </c>
       <c r="S5" t="n">
-        <v>0.452781468629837</v>
+        <v>0.46119424700737</v>
       </c>
       <c r="T5" t="n">
-        <v>0.8417201042175293</v>
+        <v>0.8388619422912598</v>
       </c>
       <c r="U5" t="n">
-        <v>0.3363668024539948</v>
+        <v>0.3428969979286194</v>
       </c>
       <c r="V5" t="n">
-        <v>0.814048171043396</v>
+        <v>0.8134418725967407</v>
       </c>
       <c r="W5" t="n">
-        <v>0.4252075552940369</v>
+        <v>0.4227980375289917</v>
       </c>
       <c r="X5" t="n">
-        <v>0.8422830700874329</v>
+        <v>0.8395548462867737</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.3322798609733582</v>
+        <v>0.3400019407272339</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.8425861597061157</v>
+        <v>0.8396847248077393</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.3339123427867889</v>
+        <v>0.3402486741542816</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.8451845049858093</v>
+        <v>0.8447514176368713</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.4042204916477203</v>
+        <v>0.4030531942844391</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.8415468335151672</v>
+        <v>0.8393815755844116</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.3322315812110901</v>
+        <v>0.3416381478309631</v>
       </c>
       <c r="AF5" t="n">
-        <v>6.732691287994385</v>
+        <v>6.813461303710938</v>
       </c>
     </row>
     <row r="6">
@@ -992,97 +992,97 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8430192470550537</v>
+        <v>0.8425428867340088</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3289691209793091</v>
+        <v>0.3289871513843536</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6643859148025513</v>
+        <v>0.6635198593139648</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8918812870979309</v>
+        <v>0.889176070690155</v>
       </c>
       <c r="F6" t="n">
-        <v>0.7792742252349854</v>
+        <v>0.7769790291786194</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5582778453826904</v>
+        <v>0.5562561750411987</v>
       </c>
       <c r="H6" t="n">
-        <v>0.63831627368927</v>
+        <v>0.6384462118148804</v>
       </c>
       <c r="I6" t="n">
-        <v>0.9025792479515076</v>
+        <v>0.9029620289802551</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8424995541572571</v>
+        <v>0.8419799208641052</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3293662071228027</v>
+        <v>0.3308498859405518</v>
       </c>
       <c r="L6" t="n">
-        <v>0.84340900182724</v>
+        <v>0.8397713303565979</v>
       </c>
       <c r="M6" t="n">
-        <v>0.3339523375034332</v>
+        <v>0.3358559906482697</v>
       </c>
       <c r="N6" t="n">
-        <v>0.8479126691818237</v>
+        <v>0.8457907438278198</v>
       </c>
       <c r="O6" t="n">
-        <v>0.3986920416355133</v>
+        <v>0.3835130333900452</v>
       </c>
       <c r="P6" t="n">
-        <v>0.8432790637016296</v>
+        <v>0.8420665264129639</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.3287070095539093</v>
+        <v>0.3294890820980072</v>
       </c>
       <c r="R6" t="n">
-        <v>0.803178608417511</v>
+        <v>0.8023557662963867</v>
       </c>
       <c r="S6" t="n">
-        <v>0.4481481909751892</v>
+        <v>0.448225349187851</v>
       </c>
       <c r="T6" t="n">
-        <v>0.8416767716407776</v>
+        <v>0.8397713303565979</v>
       </c>
       <c r="U6" t="n">
-        <v>0.3331458270549774</v>
+        <v>0.3319608867168427</v>
       </c>
       <c r="V6" t="n">
-        <v>0.816126823425293</v>
+        <v>0.8200675845146179</v>
       </c>
       <c r="W6" t="n">
-        <v>0.4213265776634216</v>
+        <v>0.3985214531421661</v>
       </c>
       <c r="X6" t="n">
-        <v>0.8436254858970642</v>
+        <v>0.8406807780265808</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.3274954557418823</v>
+        <v>0.3291098177433014</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.8424995541572571</v>
+        <v>0.8415468335151672</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.3298241794109344</v>
+        <v>0.3297704458236694</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.8474796414375305</v>
+        <v>0.8454009890556335</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.3992651700973511</v>
+        <v>0.3842870593070984</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.8425861597061157</v>
+        <v>0.8428027033805847</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.3282879292964935</v>
+        <v>0.3300549983978271</v>
       </c>
       <c r="AF6" t="n">
-        <v>6.659918785095215</v>
+        <v>6.609016418457031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>